<commit_message>
Ich habe die Gliederung angepasst.
</commit_message>
<xml_diff>
--- a/Gliederung - Quellen die ich verwenden will.xlsx
+++ b/Gliederung - Quellen die ich verwenden will.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D71C63-924C-49DD-A72C-182307C66651}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B691FD43-D45B-4CAB-A42B-78342383B9FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
-  <si>
-    <t>Gliederungspunk</t>
-  </si>
-  <si>
-    <t>Begründung</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>1 Einleitung</t>
   </si>
@@ -40,39 +34,21 @@
     <t>2.2 Haptische Schnittstellen</t>
   </si>
   <si>
-    <t>2.3 Uberwachungsaufgaben</t>
-  </si>
-  <si>
     <t>3 Wiederherstellung und Ersetzen von Fahigkeiten</t>
   </si>
   <si>
-    <t>3.1 Sehvermogen</t>
-  </si>
-  <si>
-    <t>3.2 Horvermogen</t>
-  </si>
-  <si>
-    <t>3.3 Sprachvermogen</t>
-  </si>
-  <si>
     <t>4 Nutzung zur Leistungssteigernd</t>
   </si>
   <si>
     <t>4.1 Erlernen von motorsichen Fagikeiten</t>
   </si>
   <si>
-    <t>4.2 Erhohung der Reaktionsgeschwindigkeit</t>
-  </si>
-  <si>
     <t>5 Erweiterung des Wahrnehmungsspektrums</t>
   </si>
   <si>
     <t>5.1 Navigationssysteme</t>
   </si>
   <si>
-    <t>5.2 Nahewahrnehmung</t>
-  </si>
-  <si>
     <t>Quellen</t>
   </si>
   <si>
@@ -104,13 +80,34 @@
   </si>
   <si>
     <t>14 - Tactual Displays for Sensory Substitution and Warable Computers</t>
+  </si>
+  <si>
+    <t>Gliederungspunkt</t>
+  </si>
+  <si>
+    <t>2.3 Überwachungsaufgaben</t>
+  </si>
+  <si>
+    <t>3.1 Sehvermögen</t>
+  </si>
+  <si>
+    <t>3.3 Sprachvermögen</t>
+  </si>
+  <si>
+    <t>5.2 Nähewahrnehmung</t>
+  </si>
+  <si>
+    <t>4.2 Erhöhung der Reaktionsgeschwindigkeit</t>
+  </si>
+  <si>
+    <t>3.2 Hörvermögen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,8 +115,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,12 +140,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -172,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -180,13 +179,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -469,144 +471,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="42" style="2" customWidth="1"/>
-    <col min="3" max="3" width="66.42578125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="4"/>
+    <col min="3" max="16384" width="11.42578125" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>